<commit_message>
UNICEF standards and z-score code
</commit_message>
<xml_diff>
--- a/data/UNICEF_standards.xlsx
+++ b/data/UNICEF_standards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Lexar/Kimetrica/NICHE/NICHE_Sampling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicampion/Documents/git_repositories/NICHE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18565,7 +18565,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18631,7 +18631,7 @@
         <v>1.8931</v>
       </c>
       <c r="F2">
-        <f>G2-E2</f>
+        <f t="shared" ref="F2:F26" si="0">G2-E2</f>
         <v>42.306900000000006</v>
       </c>
       <c r="G2">
@@ -18656,7 +18656,7 @@
         <v>55.6</v>
       </c>
       <c r="N2">
-        <f>M2+E2</f>
+        <f t="shared" ref="N2:N26" si="1">M2+E2</f>
         <v>57.493099999999998</v>
       </c>
     </row>
@@ -18677,7 +18677,7 @@
         <v>1.9464999999999999</v>
       </c>
       <c r="F3">
-        <f>G3-E3</f>
+        <f t="shared" si="0"/>
         <v>46.953499999999998</v>
       </c>
       <c r="G3">
@@ -18702,7 +18702,7 @@
         <v>60.6</v>
       </c>
       <c r="N3">
-        <f>M3+E3</f>
+        <f t="shared" si="1"/>
         <v>62.546500000000002</v>
       </c>
     </row>
@@ -18723,7 +18723,7 @@
         <v>2.0005000000000002</v>
       </c>
       <c r="F4">
-        <f>G4-E4</f>
+        <f t="shared" si="0"/>
         <v>50.399499999999996</v>
       </c>
       <c r="G4">
@@ -18748,7 +18748,7 @@
         <v>64.400000000000006</v>
       </c>
       <c r="N4">
-        <f>M4+E4</f>
+        <f t="shared" si="1"/>
         <v>66.400500000000008</v>
       </c>
     </row>
@@ -18769,7 +18769,7 @@
         <v>2.0444</v>
       </c>
       <c r="F5">
-        <f>G5-E5</f>
+        <f t="shared" si="0"/>
         <v>53.255599999999994</v>
       </c>
       <c r="G5">
@@ -18794,7 +18794,7 @@
         <v>67.599999999999994</v>
       </c>
       <c r="N5">
-        <f>M5+E5</f>
+        <f t="shared" si="1"/>
         <v>69.64439999999999</v>
       </c>
     </row>
@@ -18815,7 +18815,7 @@
         <v>2.0808</v>
       </c>
       <c r="F6">
-        <f>G6-E6</f>
+        <f t="shared" si="0"/>
         <v>55.519199999999998</v>
       </c>
       <c r="G6">
@@ -18840,7 +18840,7 @@
         <v>70.099999999999994</v>
       </c>
       <c r="N6">
-        <f>M6+E6</f>
+        <f t="shared" si="1"/>
         <v>72.180799999999991</v>
       </c>
     </row>
@@ -18861,7 +18861,7 @@
         <v>2.1114999999999999</v>
       </c>
       <c r="F7">
-        <f>G7-E7</f>
+        <f t="shared" si="0"/>
         <v>57.488500000000002</v>
       </c>
       <c r="G7">
@@ -18886,7 +18886,7 @@
         <v>72.2</v>
       </c>
       <c r="N7">
-        <f>M7+E7</f>
+        <f t="shared" si="1"/>
         <v>74.311500000000009</v>
       </c>
     </row>
@@ -18907,7 +18907,7 @@
         <v>2.1402999999999999</v>
       </c>
       <c r="F8">
-        <f>G8-E8</f>
+        <f t="shared" si="0"/>
         <v>59.059700000000007</v>
       </c>
       <c r="G8">
@@ -18932,7 +18932,7 @@
         <v>74</v>
       </c>
       <c r="N8">
-        <f>M8+E8</f>
+        <f t="shared" si="1"/>
         <v>76.140299999999996</v>
       </c>
     </row>
@@ -18953,7 +18953,7 @@
         <v>2.1711</v>
       </c>
       <c r="F9">
-        <f>G9-E9</f>
+        <f t="shared" si="0"/>
         <v>60.5289</v>
       </c>
       <c r="G9">
@@ -18978,7 +18978,7 @@
         <v>75.7</v>
       </c>
       <c r="N9">
-        <f>M9+E9</f>
+        <f t="shared" si="1"/>
         <v>77.871099999999998</v>
       </c>
     </row>
@@ -18999,7 +18999,7 @@
         <v>2.2054999999999998</v>
       </c>
       <c r="F10">
-        <f>G10-E10</f>
+        <f t="shared" si="0"/>
         <v>61.794499999999999</v>
       </c>
       <c r="G10">
@@ -19024,7 +19024,7 @@
         <v>77.2</v>
       </c>
       <c r="N10">
-        <f>M10+E10</f>
+        <f t="shared" si="1"/>
         <v>79.405500000000004</v>
       </c>
     </row>
@@ -19045,7 +19045,7 @@
         <v>2.2433000000000001</v>
       </c>
       <c r="F11">
-        <f>G11-E11</f>
+        <f t="shared" si="0"/>
         <v>62.956700000000005</v>
       </c>
       <c r="G11">
@@ -19070,7 +19070,7 @@
         <v>78.7</v>
       </c>
       <c r="N11">
-        <f>M11+E11</f>
+        <f t="shared" si="1"/>
         <v>80.943300000000008</v>
       </c>
     </row>
@@ -19091,7 +19091,7 @@
         <v>2.2848999999999999</v>
       </c>
       <c r="F12">
-        <f>G12-E12</f>
+        <f t="shared" si="0"/>
         <v>64.115100000000012</v>
       </c>
       <c r="G12">
@@ -19116,7 +19116,7 @@
         <v>80.099999999999994</v>
       </c>
       <c r="N12">
-        <f>M12+E12</f>
+        <f t="shared" si="1"/>
         <v>82.384899999999988</v>
       </c>
     </row>
@@ -19137,7 +19137,7 @@
         <v>2.3292999999999999</v>
       </c>
       <c r="F13">
-        <f>G13-E13</f>
+        <f t="shared" si="0"/>
         <v>65.270699999999991</v>
       </c>
       <c r="G13">
@@ -19162,7 +19162,7 @@
         <v>81.5</v>
       </c>
       <c r="N13">
-        <f>M13+E13</f>
+        <f t="shared" si="1"/>
         <v>83.829300000000003</v>
       </c>
     </row>
@@ -19183,7 +19183,7 @@
         <v>2.3761999999999999</v>
       </c>
       <c r="F14">
-        <f>G14-E14</f>
+        <f t="shared" si="0"/>
         <v>66.223799999999997</v>
       </c>
       <c r="G14">
@@ -19208,7 +19208,7 @@
         <v>82.9</v>
       </c>
       <c r="N14">
-        <f>M14+E14</f>
+        <f t="shared" si="1"/>
         <v>85.276200000000003</v>
       </c>
     </row>
@@ -19229,7 +19229,7 @@
         <v>2.4260000000000002</v>
       </c>
       <c r="F15">
-        <f>G15-E15</f>
+        <f t="shared" si="0"/>
         <v>67.173999999999992</v>
       </c>
       <c r="G15">
@@ -19254,7 +19254,7 @@
         <v>84.2</v>
       </c>
       <c r="N15">
-        <f>M15+E15</f>
+        <f t="shared" si="1"/>
         <v>86.626000000000005</v>
       </c>
     </row>
@@ -19275,7 +19275,7 @@
         <v>2.4773000000000001</v>
       </c>
       <c r="F16">
-        <f>G16-E16</f>
+        <f t="shared" si="0"/>
         <v>68.122699999999995</v>
       </c>
       <c r="G16">
@@ -19300,7 +19300,7 @@
         <v>85.5</v>
       </c>
       <c r="N16">
-        <f>M16+E16</f>
+        <f t="shared" si="1"/>
         <v>87.9773</v>
       </c>
     </row>
@@ -19321,7 +19321,7 @@
         <v>2.5303</v>
       </c>
       <c r="F17">
-        <f>G17-E17</f>
+        <f t="shared" si="0"/>
         <v>69.069699999999997</v>
       </c>
       <c r="G17">
@@ -19346,7 +19346,7 @@
         <v>86.7</v>
       </c>
       <c r="N17">
-        <f>M17+E17</f>
+        <f t="shared" si="1"/>
         <v>89.2303</v>
       </c>
     </row>
@@ -19367,7 +19367,7 @@
         <v>2.5844</v>
       </c>
       <c r="F18">
-        <f>G18-E18</f>
+        <f t="shared" si="0"/>
         <v>69.915599999999998</v>
       </c>
       <c r="G18">
@@ -19392,7 +19392,7 @@
         <v>88</v>
       </c>
       <c r="N18">
-        <f>M18+E18</f>
+        <f t="shared" si="1"/>
         <v>90.584400000000002</v>
       </c>
     </row>
@@ -19413,7 +19413,7 @@
         <v>2.6406000000000001</v>
       </c>
       <c r="F19">
-        <f>G19-E19</f>
+        <f t="shared" si="0"/>
         <v>70.659399999999991</v>
       </c>
       <c r="G19">
@@ -19438,7 +19438,7 @@
         <v>89.2</v>
       </c>
       <c r="N19">
-        <f>M19+E19</f>
+        <f t="shared" si="1"/>
         <v>91.840600000000009</v>
       </c>
     </row>
@@ -19459,7 +19459,7 @@
         <v>2.6972999999999998</v>
       </c>
       <c r="F20">
-        <f>G20-E20</f>
+        <f t="shared" si="0"/>
         <v>71.502700000000004</v>
       </c>
       <c r="G20">
@@ -19484,7 +19484,7 @@
         <v>90.4</v>
       </c>
       <c r="N20">
-        <f>M20+E20</f>
+        <f t="shared" si="1"/>
         <v>93.097300000000004</v>
       </c>
     </row>
@@ -19505,7 +19505,7 @@
         <v>2.7553000000000001</v>
       </c>
       <c r="F21">
-        <f>G21-E21</f>
+        <f t="shared" si="0"/>
         <v>72.244699999999995</v>
       </c>
       <c r="G21">
@@ -19530,7 +19530,7 @@
         <v>91.5</v>
       </c>
       <c r="N21">
-        <f>M21+E21</f>
+        <f t="shared" si="1"/>
         <v>94.255300000000005</v>
       </c>
     </row>
@@ -19551,7 +19551,7 @@
         <v>2.8140000000000001</v>
       </c>
       <c r="F22">
-        <f>G22-E22</f>
+        <f t="shared" si="0"/>
         <v>72.98599999999999</v>
       </c>
       <c r="G22">
@@ -19576,7 +19576,7 @@
         <v>92.6</v>
       </c>
       <c r="N22">
-        <f>M22+E22</f>
+        <f t="shared" si="1"/>
         <v>95.413999999999987</v>
       </c>
     </row>
@@ -19597,7 +19597,7 @@
         <v>2.8742000000000001</v>
       </c>
       <c r="F23">
-        <f>G23-E23</f>
+        <f t="shared" si="0"/>
         <v>73.625799999999998</v>
       </c>
       <c r="G23">
@@ -19622,7 +19622,7 @@
         <v>93.8</v>
       </c>
       <c r="N23">
-        <f>M23+E23</f>
+        <f t="shared" si="1"/>
         <v>96.674199999999999</v>
       </c>
     </row>
@@ -19643,7 +19643,7 @@
         <v>2.9342000000000001</v>
       </c>
       <c r="F24">
-        <f>G24-E24</f>
+        <f t="shared" si="0"/>
         <v>74.265799999999999</v>
       </c>
       <c r="G24">
@@ -19668,7 +19668,7 @@
         <v>94.9</v>
       </c>
       <c r="N24">
-        <f>M24+E24</f>
+        <f t="shared" si="1"/>
         <v>97.83420000000001</v>
       </c>
     </row>
@@ -19689,7 +19689,7 @@
         <v>2.9950999999999999</v>
       </c>
       <c r="F25">
-        <f>G25-E25</f>
+        <f t="shared" si="0"/>
         <v>75.004900000000006</v>
       </c>
       <c r="G25">
@@ -19714,7 +19714,7 @@
         <v>95.9</v>
       </c>
       <c r="N25">
-        <f>M25+E25</f>
+        <f t="shared" si="1"/>
         <v>98.895099999999999</v>
       </c>
     </row>
@@ -19735,7 +19735,7 @@
         <v>3.0550999999999999</v>
       </c>
       <c r="F26">
-        <f>G26-E26</f>
+        <f t="shared" si="0"/>
         <v>75.644900000000007</v>
       </c>
       <c r="G26">
@@ -19760,7 +19760,7 @@
         <v>97</v>
       </c>
       <c r="N26">
-        <f>M26+E26</f>
+        <f t="shared" si="1"/>
         <v>100.0551</v>
       </c>
     </row>

</xml_diff>